<commit_message>
feat: agrega excel con matriz de estados
</commit_message>
<xml_diff>
--- a/Documentos/Matriz de transición de estados.xlsx
+++ b/Documentos/Matriz de transición de estados.xlsx
@@ -449,10 +449,10 @@
         <v>16</v>
       </c>
       <c r="I2" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="J2" s="5">
         <v>6.0</v>
-      </c>
-      <c r="J2" s="5">
-        <v>7.0</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>16</v>
@@ -706,8 +706,8 @@
       <c r="H8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="5">
-        <v>8.0</v>
+      <c r="I8" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>16</v>
@@ -759,8 +759,8 @@
       <c r="H9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>16</v>
+      <c r="I9" s="5">
+        <v>8.0</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>16</v>

</xml_diff>